<commit_message>
push THESTREAK to repo
</commit_message>
<xml_diff>
--- a/Artists/Bump,Bump,Bump.xlsx
+++ b/Artists/Bump,Bump,Bump.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['We sending this out to all the ladies all over the world']</t>
+          <t>['Hello, everyone, this is your action news reporter with all the news that is news across the nation, on the scene at the supermarket.']</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['All the ladies all over the world']</t>
+          <t>['Yeah, I did.']</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['All my sexy mamas come on']</t>
+          <t>["I's standin' overe there by the tomaters, and here he come, running through the pole beans, through the fruits and vegetables, nekkid as a jay bird."]</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['Come on a come on now']</t>
+          <t>['And I hollered over t\' Ethel, I said, "Don\'t look, Ethel!"']</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['As we proceed to give you what you need']</t>
+          <t>["But it's too late, she'd already been incensed."]</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['Bump bump bump']</t>
+          <t>['Here he comes, look at that, look at that']</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['Bad boy, b2k, yo o, talk to em player']</t>
+          <t>['There he goes, look at that, look at that']</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['I like your lil sexy style']</t>
+          <t>["And he ain't wearin' no clothes"]</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>["I love it when you getting wil' (uh, i see you)"]</t>
+          <t>['(Look at that, look at that)']</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['Girl in the club wit me']</t>
+          <t>['Of his anatomy']</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['(come over her let me talk to you for a minute, yeah']</t>
+          <t>["Invitin' public critique"]</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['I wanna tell you something)']</t>
+          <t>['Yeah, I did.']</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['Girl you need to be in magazines']</t>
+          <t>["I's just in here gettin my car checked, he just appeared out of the traffic."]</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>["Wit a crown on your head cause you's a ghetto queen"]</t>
+          <t>["Come streakin' around the grease rack there, didn't have nothin' on but a smile."]</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['Like bling bling bling (uh come on, you fine girl)']</t>
+          <t>["I looked in there, and Ethel was gettin' her a cold drink."]</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['The way you shakin that sexy (oh)']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['Body']</t>
+          <t>["She'd already been mooned."]</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>['Shaped like an hour glass (ow)']</t>
+          <t>['Flashed her right there in front of the shock absorbers.']</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['Can we spend some time']</t>
+          <t>["He ain't crude, look at that, look at that"]</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>["(yeah, lets do it ya'll)"]</t>
+          <t>["He ain't lewd, look at that, look at that"]</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['I wanna get you to myself']</t>
+          <t>['(Look at that, look at that)']</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>['You and me and nobody else']</t>
+          <t>['(Look at that, look at that)']</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>['Yo do the things we do']</t>
+          <t>["He's always makin' the news"]</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>['Baby there is something that i need from you']</t>
+          <t>["Wearin' just his tennis shoes"]</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>['And let me see that sexy body go']</t>
+          <t>['Guess you could call him unique']</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>['That is all i want to see,']</t>
+          <t>['Yeah, I did.']</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>['Baby turn around,']</t>
+          <t>["Half time, I's just goin' down thar to get Ethel a snow cone."]</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>['Bump bump bump']</t>
+          <t>['And here he come, right out of the cheap seats, dribbling, right down the middle of the court.']</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>['I can take it']</t>
+          <t>["Didn't have on nothing but his PF's."]</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>['Come on']</t>
+          <t>['Made a hook shot and got out through the concessions stand.']</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>['Girl why you teasin me']</t>
+          <t>['But it was too late.']</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>['You gonna have to stop pleasin me (stop teasin me, i want you)']</t>
+          <t>["She'd already got a free shot."]</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>["While we're on this floor"]</t>
+          <t>['(Look at that, look at that)']</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>['You takin it round and round']</t>
+          <t>['Of his anatomy']</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>['I love the way you put it down']</t>
+          <t>["He's gonna give us a peek"]</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>["You makin me scream for more (oh, gimme more, let s go, don't stop come on)"]</t>
+          <t>['Here he comes again.']</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>['Put your 2way next to mine']</t>
+          <t>["Who's that with him?"]</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>['Baby hit me anytime']</t>
+          <t>['Ethel?']</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>['Baby you and me behind close doors (oohh)']</t>
+          <t>['Is that you, Ethel?']</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>['You about to be my main squeeze']</t>
+          <t>["What do you think you're"]</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>['Take trips, cop shiny things']</t>
+          <t>["doin'?"]</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>['Girl just come wit me']</t>
+          <t>['You git your']</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>['That is all i want to see,']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>['I can take it']</t>
+          <t>["Where you goin'?"]</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>['(yeah, its bad boy baby, check this out']</t>
+          <t>['Ethel, you shameless']</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>['They call me diddy)']</t>
+          <t>['hussy!']</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>['Uh dance for nothin mami']</t>
+          <t>['Ethel!']</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>['Plans for take a mami']</t>
+          <t>['Ethelllllll!!']</t>
         </is>
       </c>
     </row>
@@ -1041,763 +1041,295 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>['Get on the floor']</t>
+          <t>['!']</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Verse 51</t>
+          <t>Pre-or-Post-Chorus 1</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>['Make it bump more']</t>
+          <t>Pardon me, sir, did you see what happened?</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Verse 52</t>
+          <t>Pre-or-Post-Chorus 2</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>['Shake it mami']</t>
+          <t>Yeah, I did.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Verse 53</t>
+          <t>Pre-or-Post-Chorus 3</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>['Lets ride']</t>
+          <t>He's just as proud as he can be</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Verse 54</t>
+          <t>Pre-or-Post-Chorus 4</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>['Im your clyde']</t>
+          <t>Of his anatomy</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Verse 55</t>
+          <t>Pre-or-Post-Chorus 5</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>['You can be my bonnie']</t>
+          <t>He likes to show off his physique</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Verse 56</t>
+          <t>Pre-or-Post-Chorus 6</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>['See you type for me']</t>
+          <t>If there's an audience to be found</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Verse 57</t>
+          <t>Pre-or-Post-Chorus 7</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>['Mami so right for me']</t>
+          <t>He'll be streakin' around</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Verse 58</t>
+          <t>Pre-or-Post-Chorus 8</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>['Man she can move it']</t>
+          <t>Invitin' public critique</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Verse 59</t>
+          <t>Pre-or-Post-Chorus 9</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>['Love when she dance to the music']</t>
+          <t>But it was too late.</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Verse 60</t>
+          <t>Pre-or-Post-Chorus 10</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>['Make me wanna stand like a pool stick']</t>
+          <t>Ethel!</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Verse 61</t>
+          <t>Chorus 1</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>['Hands is the smoothest just a simple touch make me lose it']</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Verse 62</t>
+          <t>Chorus 2</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>["Girl, that's enough"]</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Verse 63</t>
+          <t>Chorus 3</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>Oh, yes, they call him the Streak</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Verse 64</t>
+          <t>Chorus 4</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>['I pump that']</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Verse 65</t>
+          <t>Chorus 5</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>['Bump that']</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Verse 66</t>
+          <t>Chorus 6</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>['I want that']</t>
+          <t>Oh, yes, they call him the Streak</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Verse 67</t>
+          <t>Chorus 7</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>['Du du du du duda du du du']</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Verse 68</t>
+          <t>Chorus 8</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>['So lets do it again mami']</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Verse 69</t>
+          <t>Chorus 9</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>['You and a friend mami']</t>
+          <t>Oh, yes, they call him the Streak</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Verse 70</t>
+          <t>Chorus 10</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>['Money aint a thing mami']</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Verse 71</t>
+          <t>Chorus 11</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>['What i gotta spend mami']</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Verse 72</t>
+          <t>Chorus 12</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>['Put up you hands for me']</t>
+          <t>Oh, yes, they call him the Streak</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Verse 73</t>
+          <t>Chorus 13</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>["That's how you dance for me"]</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Verse 74</t>
+          <t>Chorus 14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>['Shake it like you can hunni']</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Verse 75</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>['Baby turn around,']</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Verse 76</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>['That is all i want to see,']</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Verse 77</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>['Baby show me (let me ya)']</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Verse 78</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>['Baby turn around, (b2k)']</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Verse 79</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>['And let me see that sexy body go (bad boy)']</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Verse 80</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>['I can take it']</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Verse 81</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>['I see you chris']</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Verse 82</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>['Bump bump bump']</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Verse 83</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>["Don't stop"]</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Verse 84</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>['Lets go, lets go']</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Verse 85</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>['Lets go']</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Verse 86</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>['And another one']</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Verse 87</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>['Its pandamonium baby']</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Pre-or-Post-Chorus 1</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>The way you throwin that thing at me</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Pre-or-Post-Chorus 2</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Bump that</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Pre-or-Post-Chorus 3</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Du du du du duda du du du</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>Pre-or-Post-Chorus 4</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>C'mon</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>Pre-or-Post-Chorus 5</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Lets go</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>Chorus 1</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Bump bump bump</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>Chorus 2</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Baby turn around,</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>Chorus 3</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>And let me see that sexy body go</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>Chorus 4</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>That is all i want to see,</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>Chorus 5</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Baby turn around,</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>Chorus 6</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Bump bump bump</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>Chorus 7</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>I can take it</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>Chorus 8</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Baby turn around,</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>Chorus 9</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>And let me see that sexy body go</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>Chorus 10</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Bump bump bump</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>Chorus 11</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>That is all i want to see,</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>Chorus 12</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Baby turn around,</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>Chorus 13</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>And let me see that sexy body go</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>Chorus 14</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Bump bump bump</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>Chorus 15</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>I can take it</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>Chorus 16</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Baby turn around,</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>Chorus 17</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Bump bump bump</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>Chorus 18</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>That is all i want to see,</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>Chorus 19</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>I can take it</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>Chorus 20</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Bump bump bump</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>Chorus 21</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Bump bump bump</t>
+          <t>(Look at that, look at that)</t>
         </is>
       </c>
     </row>

</xml_diff>